<commit_message>
tambah fitur import peserta
</commit_message>
<xml_diff>
--- a/public/templates/template_peserta.xlsx
+++ b/public/templates/template_peserta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\AbsenCAI\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923E14BA-C766-42D3-A2C3-136D3FA5BBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BA41B-D99B-4F74-9205-F1AA462EFB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nama</t>
   </si>
@@ -36,15 +36,9 @@
     <t>jenis_kelamin</t>
   </si>
   <si>
-    <t>desa_id</t>
-  </si>
-  <si>
     <t>kelompok_id</t>
   </si>
   <si>
-    <t>regu_id</t>
-  </si>
-  <si>
     <t>Udin</t>
   </si>
   <si>
@@ -55,6 +49,30 @@
   </si>
   <si>
     <t>Perempuan</t>
+  </si>
+  <si>
+    <t>regu</t>
+  </si>
+  <si>
+    <t>desa</t>
+  </si>
+  <si>
+    <t>Maroon</t>
+  </si>
+  <si>
+    <t>Biru</t>
+  </si>
+  <si>
+    <t>KM7</t>
+  </si>
+  <si>
+    <t>Batam</t>
+  </si>
+  <si>
+    <t>km7</t>
+  </si>
+  <si>
+    <t>batam</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,53 +409,53 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>